<commit_message>
added files to gitignore
</commit_message>
<xml_diff>
--- a/vajrang/Week1Calculator_Reframework/Data/Input/input.xlsx
+++ b/vajrang/Week1Calculator_Reframework/Data/Input/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\GitSpace\RPA-Developer-in-30-Days\vajrang\Week1Calculator_Reframework\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8872B9-BC25-43BC-97D1-BC1AE163CD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B338A38-0E36-411F-B2AC-E0FD3E4875E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>first</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>result</t>
   </si>
 </sst>
 </file>
@@ -360,15 +363,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,8 +381,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -389,8 +395,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -400,8 +409,11 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -411,8 +423,11 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -422,8 +437,11 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -433,8 +451,11 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -443,6 +464,9 @@
       </c>
       <c r="C7" t="s">
         <v>5</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>